<commit_message>
commit adjust layout  exit block and add room conifg with tags (#1541)
Co-authored-by: 汤永靖 <tangyongjing@thape.com.cn>
</commit_message>
<xml_diff>
--- a/AutoLoader/Contents/Support/疏散方向判断.xlsx
+++ b/AutoLoader/Contents/Support/疏散方向判断.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="37">
   <si>
     <t>房间A</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -292,6 +292,9 @@
   <si>
     <t>门的开启方向</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大堂</t>
   </si>
 </sst>
 </file>
@@ -649,10 +652,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -680,7 +684,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -697,7 +701,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -714,7 +718,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -731,7 +735,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -748,7 +752,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -765,7 +769,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -782,7 +786,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
@@ -799,7 +803,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>4</v>
       </c>
@@ -816,7 +820,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>4</v>
       </c>
@@ -833,7 +837,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>4</v>
       </c>
@@ -850,7 +854,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>4</v>
       </c>
@@ -867,7 +871,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>4</v>
       </c>
@@ -884,7 +888,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>4</v>
       </c>
@@ -901,7 +905,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>4</v>
       </c>
@@ -918,7 +922,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>4</v>
       </c>
@@ -935,7 +939,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>4</v>
       </c>
@@ -952,7 +956,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>4</v>
       </c>
@@ -969,7 +973,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>4</v>
       </c>
@@ -986,7 +990,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>4</v>
       </c>
@@ -1003,7 +1007,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>4</v>
       </c>
@@ -1020,7 +1024,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>4</v>
       </c>
@@ -1037,7 +1041,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>4</v>
       </c>
@@ -1054,7 +1058,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>4</v>
       </c>
@@ -1071,7 +1075,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>4</v>
       </c>
@@ -1088,7 +1092,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>4</v>
       </c>
@@ -1105,7 +1109,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>4</v>
       </c>
@@ -1122,7 +1126,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>4</v>
       </c>
@@ -1139,7 +1143,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>4</v>
       </c>
@@ -1156,7 +1160,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>4</v>
       </c>
@@ -1173,7 +1177,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>4</v>
       </c>
@@ -1190,7 +1194,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>4</v>
       </c>
@@ -1207,7 +1211,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>4</v>
       </c>
@@ -1224,7 +1228,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>4</v>
       </c>
@@ -1241,7 +1245,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>4</v>
       </c>
@@ -1258,7 +1262,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>4</v>
       </c>
@@ -1275,7 +1279,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>4</v>
       </c>
@@ -1292,7 +1296,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>4</v>
       </c>
@@ -1309,7 +1313,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>4</v>
       </c>
@@ -1326,7 +1330,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>4</v>
       </c>
@@ -1343,7 +1347,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>4</v>
       </c>
@@ -1360,7 +1364,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>21</v>
       </c>
@@ -1377,7 +1381,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>21</v>
       </c>
@@ -1394,7 +1398,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>20</v>
       </c>
@@ -1411,7 +1415,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>20</v>
       </c>
@@ -1428,7 +1432,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>20</v>
       </c>
@@ -1439,13 +1443,13 @@
         <v>2</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>20</v>
       </c>
@@ -1456,30 +1460,30 @@
         <v>2</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>20</v>
       </c>
@@ -1490,13 +1494,13 @@
         <v>2</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>20</v>
       </c>
@@ -1507,13 +1511,13 @@
         <v>2</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>24</v>
       </c>
@@ -1530,7 +1534,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>24</v>
       </c>
@@ -1547,7 +1551,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>23</v>
       </c>
@@ -1581,7 +1585,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>23</v>
       </c>
@@ -1598,7 +1602,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>24</v>
       </c>
@@ -1615,7 +1619,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>24</v>
       </c>
@@ -1632,7 +1636,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>23</v>
       </c>
@@ -1666,7 +1670,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>23</v>
       </c>
@@ -1683,7 +1687,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>23</v>
       </c>
@@ -1700,7 +1704,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
         <v>23</v>
       </c>
@@ -1717,7 +1721,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>23</v>
       </c>
@@ -1751,7 +1755,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
         <v>23</v>
       </c>
@@ -1768,7 +1772,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
         <v>23</v>
       </c>
@@ -1785,7 +1789,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
         <v>23</v>
       </c>
@@ -1819,7 +1823,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
         <v>23</v>
       </c>
@@ -1853,7 +1857,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
         <v>26</v>
       </c>
@@ -1870,7 +1874,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
         <v>26</v>
       </c>
@@ -1886,18 +1890,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E72">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="2层以上"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="1">
-      <filters>
-        <filter val="中庭"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:E72"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>